<commit_message>
fix mk9 barrels and adjust weights
</commit_message>
<xml_diff>
--- a/changes/9mm-barrels.xlsx
+++ b/changes/9mm-barrels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingl\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E98DA3C-F17A-401C-A0C8-A8DCB64936E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D78423-EEC1-4643-8227-FD0698F65332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>new</t>
   </si>
@@ -126,6 +126,48 @@
   </si>
   <si>
     <t>HK MP5 9x19 225mm Barrel</t>
+  </si>
+  <si>
+    <t>kak_value_line_light_tapered_melonite_ar9_76mm_9x19_barrel</t>
+  </si>
+  <si>
+    <t>KAK Value Line Light Tapered Melonite AR9 3" 9x19</t>
+  </si>
+  <si>
+    <t>cmmg_mk9_216mm_9x19_barrel</t>
+  </si>
+  <si>
+    <t>CmmG Mk9 8.5" 9x19</t>
+  </si>
+  <si>
+    <t>cmmg_mk9_229mm_9x19_barrel</t>
+  </si>
+  <si>
+    <t>CmmG Mk9 9" 9x19</t>
+  </si>
+  <si>
+    <t>cmmg_mk9_406mm_9x19_c_barrel</t>
+  </si>
+  <si>
+    <t>CmmG Mk9 16" 9x19 Carbine Length</t>
+  </si>
+  <si>
+    <t>cmmg_mk9_406mm_9x19_r_barrel</t>
+  </si>
+  <si>
+    <t>CmmG Mk9 16" 9x19 Rifle Length</t>
+  </si>
+  <si>
+    <t>cmmg_mk9_406mm_9x19_m_barrel</t>
+  </si>
+  <si>
+    <t>CmmG Mk9 16" 9x19 Mid Length</t>
+  </si>
+  <si>
+    <t>cmmg_mk9_127mm_9x19_barrel</t>
+  </si>
+  <si>
+    <t>CmmG Mk9 5" 9x19</t>
   </si>
 </sst>
 </file>
@@ -970,7 +1012,7 @@
   <dimension ref="A1:U38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1130,7 +1172,7 @@
         <v>1200</v>
       </c>
       <c r="N4" s="1">
-        <f t="shared" ref="N4:N9" si="0">C4-D4*20-E4*0.8-F4*0.6-H4*5+I4*10+J4/300</f>
+        <f t="shared" ref="N4:N17" si="0">C4-D4*20-E4*0.8-F4*0.6-H4*5+I4*10+J4/300</f>
         <v>8.4333333333333353</v>
       </c>
       <c r="P4">
@@ -1140,7 +1182,7 @@
         <v>4.5</v>
       </c>
       <c r="S4">
-        <f t="shared" ref="S4:S9" si="1">ROUND(Q4*0.02+P4+R4, 2)</f>
+        <f t="shared" ref="S4:S17" si="1">ROUND(Q4*0.02+P4+R4, 2)</f>
         <v>0.15</v>
       </c>
     </row>
@@ -1371,121 +1413,365 @@
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
+      <c r="N10" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+      <c r="A11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="1">
+        <v>8</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="E11" s="1">
+        <v>7</v>
+      </c>
+      <c r="F11" s="1">
+        <v>7</v>
+      </c>
       <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
+      <c r="H11" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="I11" s="1">
+        <v>-0.3</v>
+      </c>
+      <c r="J11" s="1">
+        <v>-300</v>
+      </c>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
+      <c r="M11" s="1">
+        <v>750</v>
+      </c>
+      <c r="N11" s="1">
+        <f t="shared" si="0"/>
+        <v>-9.7000000000000011</v>
+      </c>
+      <c r="P11">
+        <v>0.06</v>
+      </c>
+      <c r="Q11">
+        <v>3</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+      <c r="A12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="1">
+        <v>5</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.16</v>
+      </c>
+      <c r="E12" s="1">
+        <v>4</v>
+      </c>
+      <c r="F12" s="1">
+        <v>4</v>
+      </c>
       <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
+      <c r="H12" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="I12" s="1">
+        <v>-0.12</v>
+      </c>
+      <c r="J12" s="1">
+        <v>-225</v>
+      </c>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
+      <c r="M12" s="1">
+        <v>800</v>
+      </c>
+      <c r="N12" s="1">
+        <f>C12-D12*20-E12*0.8-F12*0.6-H12*5+I12*10+J12/300</f>
+        <v>-7.0000000000000009</v>
+      </c>
+      <c r="P12">
+        <v>0.06</v>
+      </c>
+      <c r="Q12">
+        <v>5</v>
+      </c>
+      <c r="S12">
+        <f>ROUND(Q12*0.02+P12+R12, 2)</f>
+        <v>0.16</v>
+      </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
+      <c r="A13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="1">
+        <v>2</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.23</v>
+      </c>
+      <c r="E13" s="1">
+        <v>2</v>
+      </c>
+      <c r="F13" s="1">
+        <v>2</v>
+      </c>
       <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
+      <c r="H13" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="I13" s="1">
+        <v>-0.04</v>
+      </c>
+      <c r="J13" s="1">
+        <v>-90</v>
+      </c>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
+      <c r="M13" s="1">
+        <v>900</v>
+      </c>
+      <c r="N13" s="1">
+        <f t="shared" si="0"/>
+        <v>-6.7000000000000011</v>
+      </c>
+      <c r="P13">
+        <v>0.06</v>
+      </c>
+      <c r="Q13">
+        <v>8.5</v>
+      </c>
+      <c r="S13">
+        <f t="shared" si="1"/>
+        <v>0.23</v>
+      </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
+      <c r="A14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0</v>
+      </c>
       <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
+      <c r="H14" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="I14" s="1">
+        <v>0</v>
+      </c>
+      <c r="J14" s="1">
+        <v>-70</v>
+      </c>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
+      <c r="M14" s="1">
+        <v>950</v>
+      </c>
+      <c r="N14" s="1">
+        <f t="shared" si="0"/>
+        <v>-5.5333333333333332</v>
+      </c>
+      <c r="P14">
+        <v>0.06</v>
+      </c>
+      <c r="Q14">
+        <v>9</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="1"/>
+        <v>0.24</v>
+      </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
+      <c r="A15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="1">
+        <v>-6</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0.38</v>
+      </c>
+      <c r="E15" s="1">
+        <v>-4</v>
+      </c>
+      <c r="F15" s="1">
+        <v>-4</v>
+      </c>
       <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
+      <c r="H15" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="J15" s="1">
+        <v>200</v>
+      </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
+      <c r="M15" s="1">
+        <v>1200</v>
+      </c>
+      <c r="N15" s="1">
+        <f t="shared" si="0"/>
+        <v>-6.5833333333333313</v>
+      </c>
+      <c r="P15">
+        <v>0.06</v>
+      </c>
+      <c r="Q15">
+        <v>16</v>
+      </c>
+      <c r="S15">
+        <f t="shared" si="1"/>
+        <v>0.38</v>
+      </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+      <c r="A16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="1">
+        <v>-7</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0.39</v>
+      </c>
+      <c r="E16" s="1">
+        <v>-5</v>
+      </c>
+      <c r="F16" s="1">
+        <v>-5</v>
+      </c>
       <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
+      <c r="H16" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="I16" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="J16" s="1">
+        <v>200</v>
+      </c>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
+      <c r="M16" s="1">
+        <v>1200</v>
+      </c>
+      <c r="N16" s="1">
+        <f t="shared" si="0"/>
+        <v>-6.3833333333333337</v>
+      </c>
+      <c r="P16">
+        <v>0.06</v>
+      </c>
+      <c r="Q16">
+        <v>16</v>
+      </c>
+      <c r="R16">
+        <v>0.01</v>
+      </c>
+      <c r="S16">
+        <f t="shared" si="1"/>
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="1">
+        <v>-8</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="E17" s="1">
+        <v>-6</v>
+      </c>
+      <c r="F17" s="1">
+        <v>-6</v>
+      </c>
       <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
+      <c r="H17" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="I17" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="J17" s="1">
+        <v>200</v>
+      </c>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M17" s="1">
+        <v>1200</v>
+      </c>
+      <c r="N17" s="1">
+        <f t="shared" si="0"/>
+        <v>-6.1833333333333327</v>
+      </c>
+      <c r="P17">
+        <v>0.06</v>
+      </c>
+      <c r="Q17">
+        <v>16</v>
+      </c>
+      <c r="R17">
+        <v>0.02</v>
+      </c>
+      <c r="S17">
+        <f t="shared" si="1"/>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1501,10 +1787,10 @@
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="N19" s="1"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1520,7 +1806,7 @@
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1536,7 +1822,7 @@
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1552,34 +1838,34 @@
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="N23" s="1"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="N24" s="1"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="N25" s="1"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="N26" s="1"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="N27" s="1"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="N28" s="1"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="N29" s="1"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="N30" s="1"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="N31" s="1"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="N32" s="1"/>
     </row>
     <row r="33" spans="14:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update pp19 barrel and weight
</commit_message>
<xml_diff>
--- a/changes/9mm-barrels.xlsx
+++ b/changes/9mm-barrels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingl\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D78423-EEC1-4643-8227-FD0698F65332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60509013-E923-4629-9738-E6B71CF60B34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>new</t>
   </si>
@@ -168,6 +168,12 @@
   </si>
   <si>
     <t>CmmG Mk9 5" 9x19</t>
+  </si>
+  <si>
+    <t>pp19_barrel</t>
+  </si>
+  <si>
+    <t>PP19 Standard</t>
   </si>
 </sst>
 </file>
@@ -1012,7 +1018,7 @@
   <dimension ref="A1:U38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1172,7 +1178,7 @@
         <v>1200</v>
       </c>
       <c r="N4" s="1">
-        <f t="shared" ref="N4:N17" si="0">C4-D4*20-E4*0.8-F4*0.6-H4*5+I4*10+J4/300</f>
+        <f t="shared" ref="N4:N19" si="0">C4-D4*20-E4*0.8-F4*0.6-H4*5+I4*10+J4/300</f>
         <v>8.4333333333333353</v>
       </c>
       <c r="P4">
@@ -1182,7 +1188,7 @@
         <v>4.5</v>
       </c>
       <c r="S4">
-        <f t="shared" ref="S4:S17" si="1">ROUND(Q4*0.02+P4+R4, 2)</f>
+        <f t="shared" ref="S4:S19" si="1">ROUND(Q4*0.02+P4+R4, 2)</f>
         <v>0.15</v>
       </c>
     </row>
@@ -1785,10 +1791,56 @@
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
+      <c r="N18" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="N19" s="1"/>
+      <c r="A19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0</v>
+      </c>
+      <c r="H19" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="I19" s="1">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>100</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19" s="1">
+        <f t="shared" si="0"/>
+        <v>-6.166666666666667</v>
+      </c>
+      <c r="P19">
+        <v>0.06</v>
+      </c>
+      <c r="Q19">
+        <v>9</v>
+      </c>
+      <c r="S19">
+        <f t="shared" si="1"/>
+        <v>0.24</v>
+      </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>

</xml_diff>

<commit_message>
a bit more aug paraing
</commit_message>
<xml_diff>
--- a/changes/9mm-barrels.xlsx
+++ b/changes/9mm-barrels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingl\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{816851E2-1A8C-45F2-967B-A9D42BF874A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{438D6759-BA52-484F-B472-30FA17C5B631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1030,7 +1030,7 @@
   <dimension ref="A1:U38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1897,10 +1897,10 @@
         <v>0.46</v>
       </c>
       <c r="E21" s="1">
-        <v>-13</v>
+        <v>-12</v>
       </c>
       <c r="F21" s="1">
-        <v>-15</v>
+        <v>-14</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1">
@@ -1919,7 +1919,7 @@
       </c>
       <c r="N21" s="1">
         <f t="shared" si="0"/>
-        <v>13.433333333333332</v>
+        <v>12.033333333333333</v>
       </c>
       <c r="P21">
         <v>0.08</v>
@@ -1940,7 +1940,7 @@
         <v>50</v>
       </c>
       <c r="C22" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D22" s="1">
         <v>0.37</v>
@@ -1949,7 +1949,7 @@
         <v>-10</v>
       </c>
       <c r="F22" s="1">
-        <v>-8</v>
+        <v>-9</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1">
@@ -1968,7 +1968,7 @@
       </c>
       <c r="N22" s="1">
         <f t="shared" si="0"/>
-        <v>10.499999999999998</v>
+        <v>9.1</v>
       </c>
       <c r="P22">
         <v>0.08</v>

</xml_diff>

<commit_message>
more aug para weirdness
</commit_message>
<xml_diff>
--- a/changes/9mm-barrels.xlsx
+++ b/changes/9mm-barrels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingl\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{438D6759-BA52-484F-B472-30FA17C5B631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E712A72A-055F-43CD-AAAF-6A86B4E54A2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1030,7 +1030,7 @@
   <dimension ref="A1:U38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1946,10 +1946,10 @@
         <v>0.37</v>
       </c>
       <c r="E22" s="1">
-        <v>-10</v>
+        <v>-9</v>
       </c>
       <c r="F22" s="1">
-        <v>-9</v>
+        <v>-8</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1">
@@ -1968,7 +1968,7 @@
       </c>
       <c r="N22" s="1">
         <f t="shared" si="0"/>
-        <v>9.1</v>
+        <v>7.6999999999999993</v>
       </c>
       <c r="P22">
         <v>0.08</v>

</xml_diff>

<commit_message>
buff mk9 a little
</commit_message>
<xml_diff>
--- a/changes/9mm-barrels.xlsx
+++ b/changes/9mm-barrels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingl\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E712A72A-055F-43CD-AAAF-6A86B4E54A2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAEE323D-7D41-4F78-9113-05C11BD4B6C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1030,7 +1030,7 @@
   <dimension ref="A1:U38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1450,16 +1450,16 @@
         <v>32</v>
       </c>
       <c r="C11" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D11" s="1">
         <v>0.13</v>
       </c>
       <c r="E11" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F11" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1">
@@ -1478,7 +1478,7 @@
       </c>
       <c r="N11" s="1">
         <f t="shared" si="0"/>
-        <v>-9.9</v>
+        <v>-10.3</v>
       </c>
       <c r="P11">
         <v>0.06</v>
@@ -1499,16 +1499,16 @@
         <v>44</v>
       </c>
       <c r="C12" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D12" s="1">
         <v>0.18</v>
       </c>
       <c r="E12" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F12" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1">
@@ -1527,7 +1527,7 @@
       </c>
       <c r="N12" s="1">
         <f>C12-D12*20-E12*0.8-F12*0.6-H12*5+I12*10+J12/300</f>
-        <v>-7.3999999999999995</v>
+        <v>-8.1999999999999993</v>
       </c>
       <c r="P12">
         <v>0.06</v>
@@ -1548,13 +1548,13 @@
         <v>34</v>
       </c>
       <c r="C13" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D13" s="1">
         <v>0.26</v>
       </c>
       <c r="E13" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F13" s="1">
         <v>2</v>
@@ -1576,7 +1576,7 @@
       </c>
       <c r="N13" s="1">
         <f t="shared" si="0"/>
-        <v>-7.3000000000000007</v>
+        <v>-7.1000000000000005</v>
       </c>
       <c r="P13">
         <v>0.06</v>
@@ -1597,16 +1597,16 @@
         <v>36</v>
       </c>
       <c r="C14" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D14" s="1">
         <v>0.27</v>
       </c>
       <c r="E14" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F14" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1">
@@ -1625,7 +1625,7 @@
       </c>
       <c r="N14" s="1">
         <f t="shared" si="0"/>
-        <v>-6.1333333333333337</v>
+        <v>-6.9333333333333336</v>
       </c>
       <c r="P14">
         <v>0.06</v>
@@ -1646,16 +1646,16 @@
         <v>38</v>
       </c>
       <c r="C15" s="1">
-        <v>-6</v>
+        <v>-3</v>
       </c>
       <c r="D15" s="1">
         <v>0.43</v>
       </c>
       <c r="E15" s="1">
-        <v>-4</v>
+        <v>-2</v>
       </c>
       <c r="F15" s="1">
-        <v>-4</v>
+        <v>-2</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1">
@@ -1674,7 +1674,7 @@
       </c>
       <c r="N15" s="1">
         <f t="shared" si="0"/>
-        <v>-7.5833333333333313</v>
+        <v>-7.3833333333333337</v>
       </c>
       <c r="P15">
         <v>0.06</v>
@@ -1695,16 +1695,16 @@
         <v>40</v>
       </c>
       <c r="C16" s="1">
-        <v>-7</v>
+        <v>-4</v>
       </c>
       <c r="D16" s="1">
         <v>0.44</v>
       </c>
       <c r="E16" s="1">
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="F16" s="1">
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1">
@@ -1723,7 +1723,7 @@
       </c>
       <c r="N16" s="1">
         <f t="shared" si="0"/>
-        <v>-7.3833333333333337</v>
+        <v>-7.1833333333333345</v>
       </c>
       <c r="P16">
         <v>0.06</v>
@@ -1747,16 +1747,16 @@
         <v>42</v>
       </c>
       <c r="C17" s="1">
-        <v>-8</v>
+        <v>-5</v>
       </c>
       <c r="D17" s="1">
         <v>0.45</v>
       </c>
       <c r="E17" s="1">
-        <v>-6</v>
+        <v>-4</v>
       </c>
       <c r="F17" s="1">
-        <v>-6</v>
+        <v>-4</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1">
@@ -1775,7 +1775,7 @@
       </c>
       <c r="N17" s="1">
         <f t="shared" si="0"/>
-        <v>-7.1833333333333327</v>
+        <v>-6.9833333333333334</v>
       </c>
       <c r="P17">
         <v>0.06</v>

</xml_diff>